<commit_message>
improvement & split multilines
</commit_message>
<xml_diff>
--- a/resources/data.xlsx
+++ b/resources/data.xlsx
@@ -16,7 +16,7 @@
     <sheet name="recommendations" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ActualizacionSO!$B$1:$F$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ActualizacionSO!$A$1:$F$52</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">recommendations!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -28,112 +28,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>tc={C411DEC1-B4D0-4B58-A355-72A7617B71ED}</author>
-    <author>tc={787F0D5F-8AF7-4285-8997-9B754DF7011C}</author>
-    <author>tc={ACEE74AA-30AB-4853-8DF5-AAA2FD866200}</author>
-    <author>tc={7B85EAF7-82FD-4DE1-8BAC-0F6572884977}</author>
-    <author>tc={6BE96759-6B12-4E77-ADBB-9EDA6AB352D7}</author>
-  </authors>
-  <commentList>
-    <comment ref="B2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Revisar el SO H
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D4" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Recomendacion [1] puesta en la pestaña de Generales
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C6" authorId="2" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Recomendacion [2] puesta en la pestaña de Generales
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C16" authorId="3" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Las recomendaciones estaban en español
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C21" authorId="4" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Recomendacion puesta en la pestaña de Generales
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="121">
   <si>
     <t>Programming Fundamentals</t>
   </si>
@@ -264,9 +160,6 @@
     <t>Desarrollo de Aplicaciones Web</t>
   </si>
   <si>
-    <t>Information System</t>
-  </si>
-  <si>
     <t>Sistemas de Información</t>
   </si>
   <si>
@@ -312,9 +205,6 @@
     <t>Ingeniería de Software II</t>
   </si>
   <si>
-    <t>Problem Solving using Applied Computer Sciences </t>
-  </si>
-  <si>
     <t>idx</t>
   </si>
   <si>
@@ -334,9 +224,6 @@
   </si>
   <si>
     <t>formation</t>
-  </si>
-  <si>
-    <t>assesment</t>
   </si>
   <si>
     <t>- At the beginning of these topic, an introduction of predicate calculus should be delivered to the students, and basic exercises should be apply, so the students feel comfortable with that knowledge forgotten 
@@ -430,10 +317,6 @@
     <t>Change the rubric’s second criterion</t>
   </si>
   <si>
-    <t>- Programming courses that are at the initial level should empathize the importance of quality assurance as part of software development fundamentals. These courses should use tools to evaluate the quality of code generated by students to improve their skills to produce high quality software.
-- Use case studies of ethical dilemma in classes to identify ethical problems, consequences, direct and indirect interested parties. Students need to face real problems of ethical dilemma to comprehend ethical and professional responsibility[2]</t>
-  </si>
-  <si>
     <t>- Analyze different tools to evaluate software quality and use the best skills to measure development fundamentals. 
 - If a group project is used to measure the ability to design a program. It is suggested to introduce some extra independent modules and assign each of these modules to each student, in order to clearly identify the work of every student.
 - Review the rubric to improve the assessment of the criterion 2</t>
@@ -524,16 +407,6 @@
 Complement the measurement of criterion 3 by asking students, as a form to defend their design, to formulate a question that the computational solution may answer in another context or in the future.</t>
   </si>
   <si>
-    <t>Use real cases in English
-Review and correct your reports as well as your presentations
-Send reading tasks about articles in newspapers of the first world of technology.
-Hacer más ejercicios durante el curso con los presentados en esta medición.
-Identificar a los estudiantes que están en desarrollo para que mejoren su
-habilidad de comunicación.
-Motivar a los estudiantes que en el manejo de proyectos, la comunicación forma_x000D_
-parte de éxito del mismo.</t>
-  </si>
-  <si>
     <t>Analyze real cases about the application of technologies in society
 Send reading papers in first world newspapers about technology applications
 Realizar dos mediciones uno al inicio y otro al final del curso, para notar la_x000D_
@@ -543,30 +416,9 @@
     <t>Discrete Mathematics</t>
   </si>
   <si>
-    <t>Methodology of Research in Computing</t>
-  </si>
-  <si>
-    <t>Information Assurance and Security</t>
-  </si>
-  <si>
-    <t>Data structures</t>
-  </si>
-  <si>
-    <t>Distributed systems</t>
-  </si>
-  <si>
     <t>Software Design</t>
   </si>
   <si>
-    <t>COMPUTER ENGINEERING CAPSTONE COURSE</t>
-  </si>
-  <si>
-    <t>Problem Solving Using Applied Computer Science</t>
-  </si>
-  <si>
-    <t>Web Application Development</t>
-  </si>
-  <si>
     <t>Analysis of Algorithms</t>
   </si>
   <si>
@@ -585,7 +437,24 @@
     <t>assessment</t>
   </si>
   <si>
-    <t>-</t>
+    <t>Problem Solving using Applied  Computer Sciences </t>
+  </si>
+  <si>
+    <t>- Programming courses that are at the initial level should empathize the importance of quality assurance as part of software development fundamentals. These courses should use tools to evaluate the quality of code generated by students to improve their skills to produce high quality software.
+- Use case studies of ethical dilemma in classes to identify ethical problems, consequences, direct and indirect interested parties. Students need to face real problems of ethical dilemma to comprehend ethical and professional responsibility</t>
+  </si>
+  <si>
+    <t>Capstone Course</t>
+  </si>
+  <si>
+    <t>Use real cases
+Review and correct reports and presentations
+Send reading tasks about articles in newspapers of the first world of technology.
+Identify students in developing stage to improve their communication skills.
+Motivate students that in project management, communication is part of project success.</t>
+  </si>
+  <si>
+    <t>"-"</t>
   </si>
 </sst>
 </file>
@@ -640,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -655,14 +524,20 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -944,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -958,62 +833,56 @@
     <col min="6" max="6" width="34.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
         <v>60</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>61</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>62</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <f>IF(B2=B3,A2,A2+1)</f>
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -1025,58 +894,58 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <f t="shared" ref="A4:A52" si="0">IF(B3=B4,A3,A3+1)</f>
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
-      </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f>IF(B5=B6,A5,A5+1)</f>
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
+        <v>33</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1088,16 +957,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
+        <v>33</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -1109,157 +978,157 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8">
         <v>3</v>
       </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8">
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
         <v>7</v>
       </c>
-      <c r="E8" t="s">
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
         <v>10</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <f t="shared" si="0"/>
         <v>7</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12">
-        <v>6</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>6</v>
       </c>
       <c r="B15" t="s">
         <v>23</v>
@@ -1268,34 +1137,34 @@
         <v>24</v>
       </c>
       <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="E15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
       <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F16" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -1304,10 +1173,10 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="D17">
         <v>7</v>
@@ -1325,19 +1194,19 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -1346,19 +1215,19 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="D19">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="F19" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -1367,19 +1236,19 @@
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -1388,19 +1257,19 @@
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -1409,19 +1278,19 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
         <v>3</v>
-      </c>
-      <c r="E22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -1430,10 +1299,10 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D23">
         <v>4</v>
@@ -1448,22 +1317,22 @@
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F24" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -1472,40 +1341,40 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>112</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F26" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -1514,10 +1383,10 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" t="s">
-        <v>36</v>
+        <v>112</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="D27">
         <v>5</v>
@@ -1535,19 +1404,19 @@
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" t="s">
-        <v>36</v>
+        <v>112</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="D28">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>21</v>
-      </c>
-      <c r="F28" t="s">
-        <v>22</v>
+        <v>10</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -1556,19 +1425,19 @@
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -1577,40 +1446,40 @@
         <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="D30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -1619,82 +1488,82 @@
         <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E32" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F32" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B33" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" t="s">
-        <v>42</v>
-      </c>
-      <c r="D33">
-        <v>2</v>
-      </c>
-      <c r="E33" t="s">
-        <v>2</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="B34" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34">
+      <c r="E34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34">
+      <c r="B35" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35">
         <v>7</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>10</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F35" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B35" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35">
-        <v>3</v>
-      </c>
-      <c r="E35" t="s">
-        <v>17</v>
-      </c>
-      <c r="F35" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -1703,19 +1572,19 @@
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>44</v>
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1</v>
       </c>
       <c r="D36">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -1724,19 +1593,19 @@
         <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>44</v>
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
       </c>
       <c r="D37">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E37" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>11</v>
+        <v>4</v>
+      </c>
+      <c r="F37" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -1745,19 +1614,19 @@
         <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F38" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -1766,40 +1635,40 @@
         <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D39">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F39" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40" t="s">
         <v>17</v>
       </c>
-      <c r="B40" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40">
-        <v>5</v>
-      </c>
-      <c r="E40" t="s">
-        <v>4</v>
-      </c>
       <c r="F40" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -1808,19 +1677,19 @@
         <v>18</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C41" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E41" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F41" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -1829,19 +1698,19 @@
         <v>18</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C42" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D42">
+        <v>5</v>
+      </c>
+      <c r="E42" t="s">
         <v>4</v>
       </c>
-      <c r="E42" t="s">
-        <v>8</v>
-      </c>
       <c r="F42" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -1850,19 +1719,19 @@
         <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C43" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D43">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E43" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F43" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -1871,19 +1740,19 @@
         <v>19</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C44" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D44">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E44" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F44" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
@@ -1892,19 +1761,19 @@
         <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D45">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F45" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
@@ -1913,19 +1782,19 @@
         <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D46">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E46" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F46" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
@@ -1934,19 +1803,19 @@
         <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C47" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E47" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F47" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
@@ -1955,10 +1824,10 @@
         <v>21</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C48" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D48">
         <v>6</v>
@@ -1976,19 +1845,19 @@
         <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="C49" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="D49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F49" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
@@ -1997,10 +1866,10 @@
         <v>22</v>
       </c>
       <c r="B50" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="C50" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="D50">
         <v>6</v>
@@ -2018,19 +1887,19 @@
         <v>23</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C51" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="E51" t="s">
+        <v>2</v>
+      </c>
+      <c r="F51" t="s">
         <v>3</v>
-      </c>
-      <c r="E51" t="s">
-        <v>17</v>
-      </c>
-      <c r="F51" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
@@ -2039,23 +1908,60 @@
         <v>23</v>
       </c>
       <c r="B52" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C52" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="D52">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E52" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F52" t="s">
-        <v>22</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>24</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F54" s="4"/>
+      <c r="A54">
+        <v>25</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>120</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2064,399 +1970,402 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.90625" style="7"/>
-    <col min="2" max="2" width="41.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.81640625" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="27.453125" style="7" customWidth="1"/>
     <col min="6" max="16384" width="10.90625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>105</v>
+      <c r="B2" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>108</v>
+      <c r="B3" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>78</v>
+        <v>24</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>120</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>90</v>
+      <c r="B6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>83</v>
+      <c r="B7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>128</v>
+      <c r="B8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>128</v>
+        <v>25</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>78</v>
+        <v>8</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>128</v>
+        <v>9</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
-        <v>12</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>78</v>
+        <v>11</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
-        <v>13</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>128</v>
+        <v>12</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
-        <v>15</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>102</v>
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
-        <v>16</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>128</v>
+        <v>15</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
-        <v>17</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>128</v>
+        <v>16</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
-        <v>19</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>78</v>
+        <v>18</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
-        <v>21</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>128</v>
+        <v>19</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
-        <v>22</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>128</v>
+        <v>20</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
+        <v>21</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="6">
+        <v>22</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="6">
         <v>23</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" s="6" t="s">
+      <c r="B22" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>128</v>
+      <c r="D22" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1">
     <sortState ref="A2:E22">
-      <sortCondition ref="A1"/>
+      <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>